<commit_message>
Minor fixes after testing on Alexa
</commit_message>
<xml_diff>
--- a/dataSamples/Fun Family Page A Day Data (v5).xlsx
+++ b/dataSamples/Fun Family Page A Day Data (v5).xlsx
@@ -45,10 +45,10 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Barry Gerhardt - Personal View" guid="{1E205BAA-3839-4793-9AC9-6DFA286FC573}" mergeInterval="0" personalView="1" xWindow="333" yWindow="59" windowWidth="1516" windowHeight="897" activeSheetId="1"/>
+    <customWorkbookView name="Windows User - Personal View" guid="{9C0311F0-DF70-44FD-BFCF-C4DBE8DC2CBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="854" activeSheetId="1"/>
+    <customWorkbookView name="Rebecca Gerhardt - Personal View" guid="{FBFDDEB8-09C3-4C2E-8A82-FA3F5F43B9A0}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1244" windowHeight="540" activeSheetId="1"/>
     <customWorkbookView name="Owner - Personal View" guid="{36663624-9048-4258-8F9E-F8388303C4CD}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="980" activeSheetId="1"/>
-    <customWorkbookView name="Rebecca Gerhardt - Personal View" guid="{FBFDDEB8-09C3-4C2E-8A82-FA3F5F43B9A0}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1244" windowHeight="540" activeSheetId="1"/>
-    <customWorkbookView name="Windows User - Personal View" guid="{9C0311F0-DF70-44FD-BFCF-C4DBE8DC2CBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="854" activeSheetId="1"/>
-    <customWorkbookView name="Barry Gerhardt - Personal View" guid="{1E205BAA-3839-4793-9AC9-6DFA286FC573}" mergeInterval="0" personalView="1" xWindow="333" yWindow="59" windowWidth="1516" windowHeight="897" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2895,13 +2895,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PAGES" displayName="PAGES" ref="A5:K428" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A5:K428">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="HOLIDAY"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:K428"/>
   <tableColumns count="11">
     <tableColumn id="1" uniqueName="ns1:TYPE" name="TYPE" dataDxfId="13">
       <xmlColumnPr mapId="1" xpath="/ns1:PAGEADAY/ns1:PAGES/ns1:PAGE/ns1:TYPE" xmlDataType="token"/>
@@ -3310,9 +3304,9 @@
   <dimension ref="A1:P428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
-      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4356,7 +4350,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <v>1</v>
       </c>
@@ -4399,7 +4393,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>518</v>
       </c>
@@ -4423,7 +4417,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>518</v>
       </c>
@@ -4447,7 +4441,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <v>1</v>
       </c>
@@ -4490,7 +4484,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C56" s="2">
         <v>1</v>
       </c>
@@ -4509,7 +4503,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C57" s="2">
         <v>1</v>
       </c>
@@ -4528,7 +4522,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C58" s="2">
         <v>1</v>
       </c>
@@ -4547,7 +4541,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C59" s="2">
         <v>1</v>
       </c>
@@ -4566,7 +4560,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C60" s="2">
         <v>1</v>
       </c>
@@ -4585,7 +4579,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C61" s="2">
         <v>1</v>
       </c>
@@ -4628,7 +4622,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>518</v>
       </c>
@@ -4652,7 +4646,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C64" s="2">
         <v>1</v>
       </c>
@@ -4695,7 +4689,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="2">
         <v>1</v>
       </c>
@@ -4714,7 +4708,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C67" s="2">
         <v>1</v>
       </c>
@@ -4733,7 +4727,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="2">
         <v>1</v>
       </c>
@@ -4776,7 +4770,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>518</v>
       </c>
@@ -4802,7 +4796,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>518</v>
       </c>
@@ -4826,7 +4820,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C72" s="2">
         <v>1</v>
       </c>
@@ -4845,7 +4839,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" s="2">
         <v>1</v>
       </c>
@@ -4864,7 +4858,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C74" s="2">
         <v>1</v>
       </c>
@@ -4883,7 +4877,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C75" s="2">
         <v>1</v>
       </c>
@@ -4902,7 +4896,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C76" s="2">
         <v>1</v>
       </c>
@@ -4921,7 +4915,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C77" s="2">
         <v>1</v>
       </c>
@@ -4964,7 +4958,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C79" s="2">
         <v>1</v>
       </c>
@@ -4983,7 +4977,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>518</v>
       </c>
@@ -5007,7 +5001,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C81" s="2">
         <v>1</v>
       </c>
@@ -5074,7 +5068,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="2">
         <v>2</v>
       </c>
@@ -5093,7 +5087,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C85" s="2">
         <v>2</v>
       </c>
@@ -5112,7 +5106,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C86" s="2">
         <v>2</v>
       </c>
@@ -5131,7 +5125,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C87" s="2">
         <v>2</v>
       </c>
@@ -5150,7 +5144,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C88" s="2">
         <v>2</v>
       </c>
@@ -5169,7 +5163,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C89" s="2">
         <v>2</v>
       </c>
@@ -5188,7 +5182,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C90" s="2">
         <v>2</v>
       </c>
@@ -5231,7 +5225,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C92" s="2">
         <v>2</v>
       </c>
@@ -5250,7 +5244,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C93" s="2">
         <v>2</v>
       </c>
@@ -5269,7 +5263,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C94" s="2">
         <v>2</v>
       </c>
@@ -5310,7 +5304,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C96" s="2">
         <v>2</v>
       </c>
@@ -5329,7 +5323,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C97" s="2">
         <v>2</v>
       </c>
@@ -5348,7 +5342,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C98" s="2">
         <v>2</v>
       </c>
@@ -5367,7 +5361,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C99" s="2">
         <v>2</v>
       </c>
@@ -5386,7 +5380,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C100" s="2">
         <v>2</v>
       </c>
@@ -5405,7 +5399,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C101" s="2">
         <v>2</v>
       </c>
@@ -5424,7 +5418,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C102" s="2">
         <v>2</v>
       </c>
@@ -5467,7 +5461,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C104" s="2">
         <v>2</v>
       </c>
@@ -5486,7 +5480,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C105" s="2">
         <v>2</v>
       </c>
@@ -5505,7 +5499,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C106" s="2">
         <v>2</v>
       </c>
@@ -5524,7 +5518,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C107" s="2">
         <v>2</v>
       </c>
@@ -5543,7 +5537,7 @@
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C108" s="2">
         <v>2</v>
       </c>
@@ -5562,7 +5556,7 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>518</v>
       </c>
@@ -5610,7 +5604,7 @@
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C111" s="2">
         <v>3</v>
       </c>
@@ -5649,7 +5643,7 @@
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>518</v>
       </c>
@@ -5697,7 +5691,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C115" s="2">
         <v>3</v>
       </c>
@@ -5716,7 +5710,7 @@
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C116" s="2">
         <v>3</v>
       </c>
@@ -5735,7 +5729,7 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>518</v>
       </c>
@@ -5759,7 +5753,7 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C118" s="2">
         <v>3</v>
       </c>
@@ -5778,7 +5772,7 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C119" s="2">
         <v>3</v>
       </c>
@@ -5797,7 +5791,7 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C120" s="2">
         <v>3</v>
       </c>
@@ -5816,7 +5810,7 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C121" s="2">
         <v>3</v>
       </c>
@@ -5835,7 +5829,7 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C122" s="2">
         <v>3</v>
       </c>
@@ -5854,7 +5848,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C123" s="2">
         <v>3</v>
       </c>
@@ -5873,7 +5867,7 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C124" s="2">
         <v>3</v>
       </c>
@@ -5916,7 +5910,7 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C126" s="2">
         <v>3</v>
       </c>
@@ -5935,7 +5929,7 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C127" s="2">
         <v>3</v>
       </c>
@@ -5976,7 +5970,7 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>518</v>
       </c>
@@ -5998,7 +5992,7 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
     </row>
-    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C130" s="2">
         <v>3</v>
       </c>
@@ -6017,7 +6011,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
     </row>
-    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C131" s="2">
         <v>3</v>
       </c>
@@ -6062,7 +6056,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C133" s="2">
         <v>3</v>
       </c>
@@ -6105,7 +6099,7 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
     </row>
-    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C135" s="2">
         <v>3</v>
       </c>
@@ -6124,7 +6118,7 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
     </row>
-    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C136" s="2">
         <v>3</v>
       </c>
@@ -6143,7 +6137,7 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
     </row>
-    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C137" s="2">
         <v>3</v>
       </c>
@@ -6162,7 +6156,7 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
     </row>
-    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C138" s="2">
         <v>3</v>
       </c>
@@ -6205,7 +6199,7 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
     </row>
-    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C140" s="2">
         <v>3</v>
       </c>
@@ -6224,7 +6218,7 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
     </row>
-    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C141" s="2">
         <v>3</v>
       </c>
@@ -6246,7 +6240,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C142" s="2">
         <v>3</v>
       </c>
@@ -6265,7 +6259,7 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
     </row>
-    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>518</v>
       </c>
@@ -6337,7 +6331,7 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C146" s="2">
         <v>4</v>
       </c>
@@ -6356,7 +6350,7 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C147" s="2">
         <v>4</v>
       </c>
@@ -6375,7 +6369,7 @@
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C148" s="2">
         <v>4</v>
       </c>
@@ -6394,7 +6388,7 @@
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C149" s="2">
         <v>4</v>
       </c>
@@ -6413,7 +6407,7 @@
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C150" s="2">
         <v>4</v>
       </c>
@@ -6432,7 +6426,7 @@
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C151" s="2">
         <v>4</v>
       </c>
@@ -6451,7 +6445,7 @@
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C152" s="2">
         <v>4</v>
       </c>
@@ -6494,7 +6488,7 @@
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>518</v>
       </c>
@@ -6518,7 +6512,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="1"/>
     </row>
-    <row r="155" spans="1:11" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>518</v>
       </c>
@@ -6542,7 +6536,7 @@
       <c r="J155" s="1"/>
       <c r="K155" s="7"/>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C156" s="2">
         <v>4</v>
       </c>
@@ -6561,7 +6555,7 @@
       <c r="J156" s="1"/>
       <c r="K156" s="8"/>
     </row>
-    <row r="157" spans="1:11" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C157" s="2">
         <v>4</v>
       </c>
@@ -6580,7 +6574,7 @@
       <c r="J157" s="1"/>
       <c r="K157" s="7"/>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C158" s="2">
         <v>4</v>
       </c>
@@ -6599,7 +6593,7 @@
       <c r="J158" s="1"/>
       <c r="K158" s="8"/>
     </row>
-    <row r="159" spans="1:11" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C159" s="2">
         <v>4</v>
       </c>
@@ -6618,7 +6612,7 @@
       <c r="J159" s="1"/>
       <c r="K159" s="7"/>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C160" s="2">
         <v>4</v>
       </c>
@@ -6637,7 +6631,7 @@
       <c r="J160" s="1"/>
       <c r="K160" s="8"/>
     </row>
-    <row r="161" spans="1:11" ht="17.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C161" s="2">
         <v>4</v>
       </c>
@@ -6656,7 +6650,7 @@
       <c r="J161" s="1"/>
       <c r="K161" s="7"/>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C162" s="2">
         <v>4</v>
       </c>
@@ -6675,7 +6669,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="1"/>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C163" s="2">
         <v>4</v>
       </c>
@@ -6694,7 +6688,7 @@
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C164" s="2">
         <v>4</v>
       </c>
@@ -6737,7 +6731,7 @@
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C166" s="2">
         <v>4</v>
       </c>
@@ -6756,7 +6750,7 @@
       <c r="J166" s="1"/>
       <c r="K166" s="1"/>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>518</v>
       </c>
@@ -6780,7 +6774,7 @@
       <c r="J167" s="1"/>
       <c r="K167" s="1"/>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C168" s="2">
         <v>4</v>
       </c>
@@ -6799,7 +6793,7 @@
       <c r="J168" s="1"/>
       <c r="K168" s="1"/>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C169" s="2">
         <v>4</v>
       </c>
@@ -6818,7 +6812,7 @@
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C170" s="2">
         <v>4</v>
       </c>
@@ -6861,7 +6855,7 @@
       <c r="J171" s="1"/>
       <c r="K171" s="1"/>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C172" s="2">
         <v>4</v>
       </c>
@@ -6880,7 +6874,7 @@
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C173" s="2">
         <v>4</v>
       </c>
@@ -6919,7 +6913,7 @@
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>644</v>
       </c>
@@ -6943,7 +6937,7 @@
       <c r="J175" s="1"/>
       <c r="K175" s="1"/>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>644</v>
       </c>
@@ -6969,7 +6963,7 @@
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C177" s="2">
         <v>5</v>
       </c>
@@ -6988,7 +6982,7 @@
       <c r="J177" s="1"/>
       <c r="K177" s="1"/>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C178" s="2">
         <v>5</v>
       </c>
@@ -7079,7 +7073,7 @@
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C182" s="2">
         <v>5</v>
       </c>
@@ -7122,7 +7116,7 @@
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C184" s="2">
         <v>5</v>
       </c>
@@ -7141,7 +7135,7 @@
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C185" s="2">
         <v>5</v>
       </c>
@@ -7160,7 +7154,7 @@
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C186" s="2">
         <v>5</v>
       </c>
@@ -7179,7 +7173,7 @@
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C187" s="2">
         <v>5</v>
       </c>
@@ -7198,7 +7192,7 @@
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C188" s="2">
         <v>5</v>
       </c>
@@ -7217,7 +7211,7 @@
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C189" s="2">
         <v>5</v>
       </c>
@@ -7236,7 +7230,7 @@
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C190" s="2">
         <v>5</v>
       </c>
@@ -7255,7 +7249,7 @@
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>644</v>
       </c>
@@ -7279,7 +7273,7 @@
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>518</v>
       </c>
@@ -7303,7 +7297,7 @@
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C193" s="2">
         <v>5</v>
       </c>
@@ -7322,7 +7316,7 @@
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>644</v>
       </c>
@@ -7346,7 +7340,7 @@
       <c r="J194" s="1"/>
       <c r="K194" s="1"/>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C195" s="2">
         <v>5</v>
       </c>
@@ -7365,7 +7359,7 @@
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>518</v>
       </c>
@@ -7413,7 +7407,7 @@
       <c r="J197" s="1"/>
       <c r="K197" s="1"/>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C198" s="2">
         <v>5</v>
       </c>
@@ -7432,7 +7426,7 @@
       <c r="J198" s="1"/>
       <c r="K198" s="1"/>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C199" s="2">
         <v>5</v>
       </c>
@@ -7451,7 +7445,7 @@
       <c r="J199" s="1"/>
       <c r="K199" s="1"/>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C200" s="2">
         <v>5</v>
       </c>
@@ -7470,7 +7464,7 @@
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C201" s="2">
         <v>5</v>
       </c>
@@ -7489,7 +7483,7 @@
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C202" s="2">
         <v>5</v>
       </c>
@@ -7508,7 +7502,7 @@
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C203" s="2">
         <v>5</v>
       </c>
@@ -7527,7 +7521,7 @@
       <c r="J203" s="1"/>
       <c r="K203" s="1"/>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C204" s="2">
         <v>5</v>
       </c>
@@ -7546,7 +7540,7 @@
       <c r="J204" s="1"/>
       <c r="K204" s="1"/>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C205" s="2">
         <v>5</v>
       </c>
@@ -7565,7 +7559,7 @@
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C206" s="2">
         <v>5</v>
       </c>
@@ -7608,7 +7602,7 @@
       <c r="J207" s="1"/>
       <c r="K207" s="1"/>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C208" s="2">
         <v>6</v>
       </c>
@@ -7627,7 +7621,7 @@
       <c r="J208" s="1"/>
       <c r="K208" s="1"/>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C209" s="2">
         <v>6</v>
       </c>
@@ -7670,7 +7664,7 @@
       <c r="J210" s="1"/>
       <c r="K210" s="1"/>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C211" s="2">
         <v>6</v>
       </c>
@@ -7711,7 +7705,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>518</v>
       </c>
@@ -7735,7 +7729,7 @@
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C214" s="2">
         <v>6</v>
       </c>
@@ -7778,7 +7772,7 @@
       <c r="J215" s="1"/>
       <c r="K215" s="1"/>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C216" s="2">
         <v>6</v>
       </c>
@@ -7797,7 +7791,7 @@
       <c r="J216" s="1"/>
       <c r="K216" s="1"/>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C217" s="2">
         <v>6</v>
       </c>
@@ -7840,7 +7834,7 @@
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C219" s="2">
         <v>6</v>
       </c>
@@ -7859,7 +7853,7 @@
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C220" s="2">
         <v>6</v>
       </c>
@@ -7902,7 +7896,7 @@
       <c r="J221" s="1"/>
       <c r="K221" s="1"/>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>518</v>
       </c>
@@ -7926,7 +7920,7 @@
       <c r="J222" s="1"/>
       <c r="K222" s="1"/>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C223" s="2">
         <v>6</v>
       </c>
@@ -7945,7 +7939,7 @@
       <c r="J223" s="1"/>
       <c r="K223" s="1"/>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C224" s="2">
         <v>6</v>
       </c>
@@ -7964,7 +7958,7 @@
       <c r="J224" s="1"/>
       <c r="K224" s="1"/>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C225" s="2">
         <v>6</v>
       </c>
@@ -7983,7 +7977,7 @@
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C226" s="2">
         <v>6</v>
       </c>
@@ -8002,7 +7996,7 @@
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C227" s="2">
         <v>6</v>
       </c>
@@ -8045,7 +8039,7 @@
       <c r="J228" s="1"/>
       <c r="K228" s="1"/>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C229" s="2">
         <v>6</v>
       </c>
@@ -8064,7 +8058,7 @@
       <c r="J229" s="1"/>
       <c r="K229" s="1"/>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C230" s="2">
         <v>6</v>
       </c>
@@ -8083,7 +8077,7 @@
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>518</v>
       </c>
@@ -8107,7 +8101,7 @@
       <c r="J231" s="1"/>
       <c r="K231" s="1"/>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C232" s="2">
         <v>6</v>
       </c>
@@ -8150,7 +8144,7 @@
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C234" s="2">
         <v>6</v>
       </c>
@@ -8169,7 +8163,7 @@
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C235" s="2">
         <v>6</v>
       </c>
@@ -8212,7 +8206,7 @@
       <c r="J236" s="1"/>
       <c r="K236" s="1"/>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C237" s="2">
         <v>6</v>
       </c>
@@ -8255,7 +8249,7 @@
       <c r="J238" s="1"/>
       <c r="K238" s="1"/>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C239" s="2">
         <v>7</v>
       </c>
@@ -8274,7 +8268,7 @@
       <c r="J239" s="1"/>
       <c r="K239" s="1"/>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C240" s="2">
         <v>7</v>
       </c>
@@ -8317,7 +8311,7 @@
       <c r="J241" s="1"/>
       <c r="K241" s="1"/>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C242" s="2">
         <v>7</v>
       </c>
@@ -8336,7 +8330,7 @@
       <c r="J242" s="1"/>
       <c r="K242" s="1"/>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C243" s="2">
         <v>7</v>
       </c>
@@ -8421,7 +8415,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C247" s="2">
         <v>7</v>
       </c>
@@ -8440,7 +8434,7 @@
       <c r="J247" s="1"/>
       <c r="K247" s="1"/>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C248" s="2">
         <v>7</v>
       </c>
@@ -8459,7 +8453,7 @@
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C249" s="2">
         <v>7</v>
       </c>
@@ -8478,7 +8472,7 @@
       <c r="J249" s="1"/>
       <c r="K249" s="1"/>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C250" s="2">
         <v>7</v>
       </c>
@@ -8521,7 +8515,7 @@
       <c r="J251" s="1"/>
       <c r="K251" s="1"/>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C252" s="2">
         <v>7</v>
       </c>
@@ -8540,7 +8534,7 @@
       <c r="J252" s="1"/>
       <c r="K252" s="1"/>
     </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C253" s="2">
         <v>7</v>
       </c>
@@ -8559,7 +8553,7 @@
       <c r="J253" s="1"/>
       <c r="K253" s="1"/>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C254" s="2">
         <v>7</v>
       </c>
@@ -8602,7 +8596,7 @@
       <c r="J255" s="1"/>
       <c r="K255" s="1"/>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C256" s="2">
         <v>7</v>
       </c>
@@ -8621,7 +8615,7 @@
       <c r="J256" s="1"/>
       <c r="K256" s="1"/>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C257" s="2">
         <v>7</v>
       </c>
@@ -8640,7 +8634,7 @@
       <c r="J257" s="1"/>
       <c r="K257" s="1"/>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C258" s="2">
         <v>7</v>
       </c>
@@ -8659,7 +8653,7 @@
       <c r="J258" s="1"/>
       <c r="K258" s="1"/>
     </row>
-    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C259" s="2">
         <v>7</v>
       </c>
@@ -8702,7 +8696,7 @@
       <c r="J260" s="1"/>
       <c r="K260" s="1"/>
     </row>
-    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C261" s="2">
         <v>7</v>
       </c>
@@ -8721,7 +8715,7 @@
       <c r="J261" s="1"/>
       <c r="K261" s="1"/>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C262" s="2">
         <v>7</v>
       </c>
@@ -8740,7 +8734,7 @@
       <c r="J262" s="1"/>
       <c r="K262" s="1"/>
     </row>
-    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C263" s="2">
         <v>7</v>
       </c>
@@ -8759,7 +8753,7 @@
       <c r="J263" s="1"/>
       <c r="K263" s="1"/>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C264" s="2">
         <v>7</v>
       </c>
@@ -8778,7 +8772,7 @@
       <c r="J264" s="1"/>
       <c r="K264" s="1"/>
     </row>
-    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C265" s="2">
         <v>7</v>
       </c>
@@ -8821,7 +8815,7 @@
       <c r="J266" s="1"/>
       <c r="K266" s="1"/>
     </row>
-    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C267" s="2">
         <v>7</v>
       </c>
@@ -8840,7 +8834,7 @@
       <c r="J267" s="1"/>
       <c r="K267" s="1"/>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C268" s="2">
         <v>7</v>
       </c>
@@ -8859,7 +8853,7 @@
       <c r="J268" s="1"/>
       <c r="K268" s="1"/>
     </row>
-    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>518</v>
       </c>
@@ -8907,7 +8901,7 @@
       <c r="J270" s="1"/>
       <c r="K270" s="1"/>
     </row>
-    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C271" s="2">
         <v>7</v>
       </c>
@@ -8926,7 +8920,7 @@
       <c r="J271" s="1"/>
       <c r="K271" s="1"/>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C272" s="2">
         <v>8</v>
       </c>
@@ -8945,7 +8939,7 @@
       <c r="J272" s="1"/>
       <c r="K272" s="1"/>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C273" s="2">
         <v>8</v>
       </c>
@@ -8964,7 +8958,7 @@
       <c r="J273" s="1"/>
       <c r="K273" s="1"/>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C274" s="2">
         <v>8</v>
       </c>
@@ -9007,7 +9001,7 @@
       <c r="J275" s="1"/>
       <c r="K275" s="1"/>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C276" s="2">
         <v>8</v>
       </c>
@@ -9026,7 +9020,7 @@
       <c r="J276" s="1"/>
       <c r="K276" s="1"/>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C277" s="2">
         <v>8</v>
       </c>
@@ -9045,7 +9039,7 @@
       <c r="J277" s="1"/>
       <c r="K277" s="1"/>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C278" s="2">
         <v>8</v>
       </c>
@@ -9064,7 +9058,7 @@
       <c r="J278" s="1"/>
       <c r="K278" s="1"/>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C279" s="2">
         <v>8</v>
       </c>
@@ -9107,7 +9101,7 @@
       <c r="J280" s="1"/>
       <c r="K280" s="1"/>
     </row>
-    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C281" s="2">
         <v>8</v>
       </c>
@@ -9126,7 +9120,7 @@
       <c r="J281" s="1"/>
       <c r="K281" s="1"/>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C282" s="2">
         <v>8</v>
       </c>
@@ -9193,7 +9187,7 @@
       <c r="J284" s="1"/>
       <c r="K284" s="1"/>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C285" s="2">
         <v>8</v>
       </c>
@@ -9212,7 +9206,7 @@
       <c r="J285" s="1"/>
       <c r="K285" s="1"/>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C286" s="2">
         <v>8</v>
       </c>
@@ -9231,7 +9225,7 @@
       <c r="J286" s="1"/>
       <c r="K286" s="1"/>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C287" s="2">
         <v>8</v>
       </c>
@@ -9250,7 +9244,7 @@
       <c r="J287" s="1"/>
       <c r="K287" s="1"/>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C288" s="2">
         <v>8</v>
       </c>
@@ -9269,7 +9263,7 @@
       <c r="J288" s="1"/>
       <c r="K288" s="1"/>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>518</v>
       </c>
@@ -9293,7 +9287,7 @@
       <c r="J289" s="1"/>
       <c r="K289" s="1"/>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C290" s="2">
         <v>8</v>
       </c>
@@ -9312,7 +9306,7 @@
       <c r="J290" s="1"/>
       <c r="K290" s="1"/>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C291" s="2">
         <v>8</v>
       </c>
@@ -9355,7 +9349,7 @@
       <c r="J292" s="1"/>
       <c r="K292" s="1"/>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C293" s="2">
         <v>8</v>
       </c>
@@ -9374,7 +9368,7 @@
       <c r="J293" s="1"/>
       <c r="K293" s="1"/>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C294" s="2">
         <v>8</v>
       </c>
@@ -9393,7 +9387,7 @@
       <c r="J294" s="1"/>
       <c r="K294" s="1"/>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C295" s="2">
         <v>8</v>
       </c>
@@ -9412,7 +9406,7 @@
       <c r="J295" s="1"/>
       <c r="K295" s="1"/>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C296" s="2">
         <v>8</v>
       </c>
@@ -9455,7 +9449,7 @@
       <c r="J297" s="1"/>
       <c r="K297" s="1"/>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C298" s="2">
         <v>8</v>
       </c>
@@ -9474,7 +9468,7 @@
       <c r="J298" s="1"/>
       <c r="K298" s="1"/>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C299" s="2">
         <v>8</v>
       </c>
@@ -9493,7 +9487,7 @@
       <c r="J299" s="1"/>
       <c r="K299" s="1"/>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C300" s="2">
         <v>8</v>
       </c>
@@ -9532,7 +9526,7 @@
       <c r="J301" s="1"/>
       <c r="K301" s="1"/>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>518</v>
       </c>
@@ -9554,7 +9548,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C303" s="2">
         <v>8</v>
       </c>
@@ -9573,7 +9567,7 @@
       <c r="J303" s="1"/>
       <c r="K303" s="1"/>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C304" s="2">
         <v>8</v>
       </c>
@@ -9592,7 +9586,7 @@
       <c r="J304" s="1"/>
       <c r="K304" s="1"/>
     </row>
-    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C305" s="2">
         <v>9</v>
       </c>
@@ -9611,7 +9605,7 @@
       <c r="J305" s="1"/>
       <c r="K305" s="1"/>
     </row>
-    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C306" s="2">
         <v>9</v>
       </c>
@@ -9630,7 +9624,7 @@
       <c r="J306" s="1"/>
       <c r="K306" s="1"/>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C307" s="2">
         <v>9</v>
       </c>
@@ -9649,7 +9643,7 @@
       <c r="J307" s="1"/>
       <c r="K307" s="1"/>
     </row>
-    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>518</v>
       </c>
@@ -9673,7 +9667,7 @@
       <c r="J308" s="1"/>
       <c r="K308" s="1"/>
     </row>
-    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C309" s="2">
         <v>9</v>
       </c>
@@ -9716,7 +9710,7 @@
       <c r="J310" s="1"/>
       <c r="K310" s="1"/>
     </row>
-    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C311" s="2">
         <v>9</v>
       </c>
@@ -9735,7 +9729,7 @@
       <c r="J311" s="1"/>
       <c r="K311" s="1"/>
     </row>
-    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C312" s="2">
         <v>9</v>
       </c>
@@ -9754,7 +9748,7 @@
       <c r="J312" s="1"/>
       <c r="K312" s="1"/>
     </row>
-    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C313" s="2">
         <v>9</v>
       </c>
@@ -9773,7 +9767,7 @@
       <c r="J313" s="1"/>
       <c r="K313" s="1"/>
     </row>
-    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C314" s="2">
         <v>9</v>
       </c>
@@ -9816,7 +9810,7 @@
       <c r="J315" s="1"/>
       <c r="K315" s="1"/>
     </row>
-    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C316" s="2">
         <v>9</v>
       </c>
@@ -9835,7 +9829,7 @@
       <c r="J316" s="1"/>
       <c r="K316" s="1"/>
     </row>
-    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C317" s="2">
         <v>9</v>
       </c>
@@ -9878,7 +9872,7 @@
       <c r="J318" s="1"/>
       <c r="K318" s="1"/>
     </row>
-    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C319" s="2">
         <v>9</v>
       </c>
@@ -9921,7 +9915,7 @@
       <c r="J320" s="1"/>
       <c r="K320" s="1"/>
     </row>
-    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C321" s="2">
         <v>9</v>
       </c>
@@ -9940,7 +9934,7 @@
       <c r="J321" s="1"/>
       <c r="K321" s="1"/>
     </row>
-    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>518</v>
       </c>
@@ -9964,7 +9958,7 @@
       <c r="J322" s="1"/>
       <c r="K322" s="1"/>
     </row>
-    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C323" s="2">
         <v>9</v>
       </c>
@@ -9983,7 +9977,7 @@
       <c r="J323" s="1"/>
       <c r="K323" s="1"/>
     </row>
-    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C324" s="2">
         <v>9</v>
       </c>
@@ -10002,7 +9996,7 @@
       <c r="J324" s="1"/>
       <c r="K324" s="1"/>
     </row>
-    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C325" s="2">
         <v>9</v>
       </c>
@@ -10021,7 +10015,7 @@
       <c r="J325" s="1"/>
       <c r="K325" s="1"/>
     </row>
-    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C326" s="2">
         <v>9</v>
       </c>
@@ -10040,7 +10034,7 @@
       <c r="J326" s="1"/>
       <c r="K326" s="1"/>
     </row>
-    <row r="327" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C327" s="2">
         <v>9</v>
       </c>
@@ -10059,7 +10053,7 @@
       <c r="J327" s="1"/>
       <c r="K327" s="1"/>
     </row>
-    <row r="328" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C328" s="2">
         <v>9</v>
       </c>
@@ -10078,7 +10072,7 @@
       <c r="J328" s="1"/>
       <c r="K328" s="1"/>
     </row>
-    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C329" s="2">
         <v>9</v>
       </c>
@@ -10121,7 +10115,7 @@
       <c r="J330" s="1"/>
       <c r="K330" s="1"/>
     </row>
-    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C331" s="2">
         <v>9</v>
       </c>
@@ -10164,7 +10158,7 @@
       <c r="J332" s="1"/>
       <c r="K332" s="1"/>
     </row>
-    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C333" s="2">
         <v>9</v>
       </c>
@@ -10183,7 +10177,7 @@
       <c r="J333" s="1"/>
       <c r="K333" s="1"/>
     </row>
-    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C334" s="2">
         <v>9</v>
       </c>
@@ -10226,7 +10220,7 @@
       <c r="J335" s="1"/>
       <c r="K335" s="1"/>
     </row>
-    <row r="336" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C336" s="2">
         <v>10</v>
       </c>
@@ -10245,7 +10239,7 @@
       <c r="J336" s="1"/>
       <c r="K336" s="1"/>
     </row>
-    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C337" s="2">
         <v>10</v>
       </c>
@@ -10264,7 +10258,7 @@
       <c r="J337" s="1"/>
       <c r="K337" s="1"/>
     </row>
-    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C338" s="2">
         <v>10</v>
       </c>
@@ -10307,7 +10301,7 @@
       <c r="J339" s="1"/>
       <c r="K339" s="1"/>
     </row>
-    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C340" s="2">
         <v>10</v>
       </c>
@@ -10326,7 +10320,7 @@
       <c r="J340" s="1"/>
       <c r="K340" s="1"/>
     </row>
-    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C341" s="2">
         <v>10</v>
       </c>
@@ -10345,7 +10339,7 @@
       <c r="J341" s="1"/>
       <c r="K341" s="1"/>
     </row>
-    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C342" s="2">
         <v>10</v>
       </c>
@@ -10364,7 +10358,7 @@
       <c r="J342" s="1"/>
       <c r="K342" s="1"/>
     </row>
-    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C343" s="2">
         <v>10</v>
       </c>
@@ -10385,7 +10379,7 @@
       <c r="J343" s="1"/>
       <c r="K343" s="1"/>
     </row>
-    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C344" s="2">
         <v>10</v>
       </c>
@@ -10404,7 +10398,7 @@
       <c r="J344" s="1"/>
       <c r="K344" s="1"/>
     </row>
-    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>518</v>
       </c>
@@ -10428,7 +10422,7 @@
       <c r="J345" s="1"/>
       <c r="K345" s="1"/>
     </row>
-    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C346" s="2">
         <v>10</v>
       </c>
@@ -10447,7 +10441,7 @@
       <c r="J346" s="1"/>
       <c r="K346" s="1"/>
     </row>
-    <row r="347" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C347" s="2">
         <v>10</v>
       </c>
@@ -10466,7 +10460,7 @@
       <c r="J347" s="1"/>
       <c r="K347" s="1"/>
     </row>
-    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C348" s="2">
         <v>10</v>
       </c>
@@ -10485,7 +10479,7 @@
       <c r="J348" s="1"/>
       <c r="K348" s="1"/>
     </row>
-    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C349" s="2">
         <v>10</v>
       </c>
@@ -10530,7 +10524,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C351" s="2">
         <v>10</v>
       </c>
@@ -10549,7 +10543,7 @@
       <c r="J351" s="1"/>
       <c r="K351" s="1"/>
     </row>
-    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C352" s="2">
         <v>10</v>
       </c>
@@ -10568,7 +10562,7 @@
       <c r="J352" s="1"/>
       <c r="K352" s="1"/>
     </row>
-    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C353" s="2">
         <v>10</v>
       </c>
@@ -10587,7 +10581,7 @@
       <c r="J353" s="1"/>
       <c r="K353" s="1"/>
     </row>
-    <row r="354" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C354" s="2">
         <v>10</v>
       </c>
@@ -10606,7 +10600,7 @@
       <c r="J354" s="1"/>
       <c r="K354" s="1"/>
     </row>
-    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>518</v>
       </c>
@@ -10630,7 +10624,7 @@
       <c r="J355" s="1"/>
       <c r="K355" s="1"/>
     </row>
-    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C356" s="2">
         <v>10</v>
       </c>
@@ -10649,7 +10643,7 @@
       <c r="J356" s="1"/>
       <c r="K356" s="1"/>
     </row>
-    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C357" s="2">
         <v>10</v>
       </c>
@@ -10668,7 +10662,7 @@
       <c r="J357" s="1"/>
       <c r="K357" s="1"/>
     </row>
-    <row r="358" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C358" s="2">
         <v>10</v>
       </c>
@@ -10689,7 +10683,7 @@
       <c r="J358" s="1"/>
       <c r="K358" s="1"/>
     </row>
-    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C359" s="2">
         <v>10</v>
       </c>
@@ -10708,7 +10702,7 @@
       <c r="J359" s="1"/>
       <c r="K359" s="1"/>
     </row>
-    <row r="360" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>518</v>
       </c>
@@ -10734,7 +10728,7 @@
       <c r="J360" s="1"/>
       <c r="K360" s="1"/>
     </row>
-    <row r="361" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C361" s="2">
         <v>10</v>
       </c>
@@ -10753,7 +10747,7 @@
       <c r="J361" s="1"/>
       <c r="K361" s="1"/>
     </row>
-    <row r="362" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C362" s="2">
         <v>10</v>
       </c>
@@ -10772,7 +10766,7 @@
       <c r="J362" s="1"/>
       <c r="K362" s="1"/>
     </row>
-    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C363" s="2">
         <v>10</v>
       </c>
@@ -10791,7 +10785,7 @@
       <c r="J363" s="1"/>
       <c r="K363" s="1"/>
     </row>
-    <row r="364" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C364" s="2">
         <v>10</v>
       </c>
@@ -10856,7 +10850,7 @@
       <c r="J366" s="1"/>
       <c r="K366" s="1"/>
     </row>
-    <row r="367" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C367" s="2">
         <v>11</v>
       </c>
@@ -10875,7 +10869,7 @@
       <c r="J367" s="1"/>
       <c r="K367" s="1"/>
     </row>
-    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C368" s="2">
         <v>11</v>
       </c>
@@ -10894,7 +10888,7 @@
       <c r="J368" s="1"/>
       <c r="K368" s="1"/>
     </row>
-    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C369" s="2">
         <v>11</v>
       </c>
@@ -10913,7 +10907,7 @@
       <c r="J369" s="1"/>
       <c r="K369" s="1"/>
     </row>
-    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C370" s="2">
         <v>11</v>
       </c>
@@ -10932,7 +10926,7 @@
       <c r="J370" s="1"/>
       <c r="K370" s="1"/>
     </row>
-    <row r="371" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C371" s="2">
         <v>11</v>
       </c>
@@ -10951,7 +10945,7 @@
       <c r="J371" s="1"/>
       <c r="K371" s="1"/>
     </row>
-    <row r="372" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>644</v>
       </c>
@@ -10975,7 +10969,7 @@
       <c r="J372" s="1"/>
       <c r="K372" s="1"/>
     </row>
-    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C373" s="2">
         <v>11</v>
       </c>
@@ -10994,7 +10988,7 @@
       <c r="J373" s="1"/>
       <c r="K373" s="1"/>
     </row>
-    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>644</v>
       </c>
@@ -11018,7 +11012,7 @@
       <c r="J374" s="1"/>
       <c r="K374" s="1"/>
     </row>
-    <row r="375" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C375" s="2">
         <v>11</v>
       </c>
@@ -11061,7 +11055,7 @@
       <c r="J376" s="1"/>
       <c r="K376" s="1"/>
     </row>
-    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C377" s="2">
         <v>11</v>
       </c>
@@ -11104,7 +11098,7 @@
       <c r="J378" s="1"/>
       <c r="K378" s="1"/>
     </row>
-    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C379" s="2">
         <v>11</v>
       </c>
@@ -11123,7 +11117,7 @@
       <c r="J379" s="1"/>
       <c r="K379" s="1"/>
     </row>
-    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>518</v>
       </c>
@@ -11147,7 +11141,7 @@
       <c r="J380" s="1"/>
       <c r="K380" s="1"/>
     </row>
-    <row r="381" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>518</v>
       </c>
@@ -11171,7 +11165,7 @@
       <c r="J381" s="1"/>
       <c r="K381" s="1"/>
     </row>
-    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C382" s="2">
         <v>11</v>
       </c>
@@ -11190,7 +11184,7 @@
       <c r="J382" s="1"/>
       <c r="K382" s="1"/>
     </row>
-    <row r="383" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C383" s="2">
         <v>11</v>
       </c>
@@ -11209,7 +11203,7 @@
       <c r="J383" s="1"/>
       <c r="K383" s="1"/>
     </row>
-    <row r="384" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C384" s="2">
         <v>11</v>
       </c>
@@ -11252,7 +11246,7 @@
       <c r="J385" s="1"/>
       <c r="K385" s="1"/>
     </row>
-    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C386" s="2">
         <v>11</v>
       </c>
@@ -11271,7 +11265,7 @@
       <c r="J386" s="1"/>
       <c r="K386" s="1"/>
     </row>
-    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C387" s="2">
         <v>11</v>
       </c>
@@ -11290,7 +11284,7 @@
       <c r="J387" s="1"/>
       <c r="K387" s="1"/>
     </row>
-    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C388" s="2">
         <v>11</v>
       </c>
@@ -11309,7 +11303,7 @@
       <c r="J388" s="1"/>
       <c r="K388" s="1"/>
     </row>
-    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>518</v>
       </c>
@@ -11333,7 +11327,7 @@
       <c r="J389" s="1"/>
       <c r="K389" s="1"/>
     </row>
-    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C390" s="2">
         <v>11</v>
       </c>
@@ -11352,7 +11346,7 @@
       <c r="J390" s="1"/>
       <c r="K390" s="1"/>
     </row>
-    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C391" s="2">
         <v>11</v>
       </c>
@@ -11371,7 +11365,7 @@
       <c r="J391" s="1"/>
       <c r="K391" s="1"/>
     </row>
-    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C392" s="2">
         <v>11</v>
       </c>
@@ -11390,7 +11384,7 @@
       <c r="J392" s="1"/>
       <c r="K392" s="1"/>
     </row>
-    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C393" s="2">
         <v>11</v>
       </c>
@@ -11433,7 +11427,7 @@
       <c r="J394" s="1"/>
       <c r="K394" s="1"/>
     </row>
-    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>518</v>
       </c>
@@ -11457,7 +11451,7 @@
       <c r="J395" s="1"/>
       <c r="K395" s="1"/>
     </row>
-    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C396" s="2">
         <v>12</v>
       </c>
@@ -11476,7 +11470,7 @@
       <c r="J396" s="1"/>
       <c r="K396" s="1"/>
     </row>
-    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C397" s="2">
         <v>12</v>
       </c>
@@ -11495,7 +11489,7 @@
       <c r="J397" s="1"/>
       <c r="K397" s="1"/>
     </row>
-    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C398" s="2">
         <v>12</v>
       </c>
@@ -11514,7 +11508,7 @@
       <c r="J398" s="1"/>
       <c r="K398" s="1"/>
     </row>
-    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C399" s="2">
         <v>12</v>
       </c>
@@ -11533,7 +11527,7 @@
       <c r="J399" s="1"/>
       <c r="K399" s="1"/>
     </row>
-    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C400" s="2">
         <v>12</v>
       </c>
@@ -11600,7 +11594,7 @@
       <c r="J402" s="1"/>
       <c r="K402" s="1"/>
     </row>
-    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C403" s="2">
         <v>12</v>
       </c>
@@ -11619,7 +11613,7 @@
       <c r="J403" s="1"/>
       <c r="K403" s="1"/>
     </row>
-    <row r="404" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C404" s="2">
         <v>12</v>
       </c>
@@ -11638,7 +11632,7 @@
       <c r="J404" s="1"/>
       <c r="K404" s="1"/>
     </row>
-    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>518</v>
       </c>
@@ -11662,7 +11656,7 @@
       <c r="J405" s="1"/>
       <c r="K405" s="1"/>
     </row>
-    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C406" s="2">
         <v>12</v>
       </c>
@@ -11703,7 +11697,7 @@
       <c r="J407" s="1"/>
       <c r="K407" s="1"/>
     </row>
-    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C408" s="2">
         <v>12</v>
       </c>
@@ -11722,7 +11716,7 @@
       <c r="J408" s="1"/>
       <c r="K408" s="1"/>
     </row>
-    <row r="409" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C409" s="2">
         <v>12</v>
       </c>
@@ -11741,7 +11735,7 @@
       <c r="J409" s="1"/>
       <c r="K409" s="1"/>
     </row>
-    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C410" s="2">
         <v>12</v>
       </c>
@@ -11760,7 +11754,7 @@
       <c r="J410" s="1"/>
       <c r="K410" s="1"/>
     </row>
-    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C411" s="2">
         <v>12</v>
       </c>
@@ -11779,7 +11773,7 @@
       <c r="J411" s="1"/>
       <c r="K411" s="1"/>
     </row>
-    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C412" s="2">
         <v>12</v>
       </c>
@@ -11822,7 +11816,7 @@
       <c r="J413" s="1"/>
       <c r="K413" s="1"/>
     </row>
-    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C414" s="2">
         <v>12</v>
       </c>
@@ -11841,7 +11835,7 @@
       <c r="J414" s="1"/>
       <c r="K414" s="1"/>
     </row>
-    <row r="415" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C415" s="2">
         <v>12</v>
       </c>
@@ -11860,7 +11854,7 @@
       <c r="J415" s="1"/>
       <c r="K415" s="1"/>
     </row>
-    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C416" s="2">
         <v>12</v>
       </c>
@@ -11879,7 +11873,7 @@
       <c r="J416" s="1"/>
       <c r="K416" s="1"/>
     </row>
-    <row r="417" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C417" s="2">
         <v>12</v>
       </c>
@@ -11898,7 +11892,7 @@
       <c r="J417" s="1"/>
       <c r="K417" s="1"/>
     </row>
-    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C418" s="2">
         <v>12</v>
       </c>
@@ -11917,7 +11911,7 @@
       <c r="J418" s="1"/>
       <c r="K418" s="1"/>
     </row>
-    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C419" s="2">
         <v>12</v>
       </c>
@@ -12032,7 +12026,7 @@
       <c r="J423" s="1"/>
       <c r="K423" s="1"/>
     </row>
-    <row r="424" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C424" s="2">
         <v>12</v>
       </c>
@@ -12051,7 +12045,7 @@
       <c r="J424" s="1"/>
       <c r="K424" s="1"/>
     </row>
-    <row r="425" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C425" s="2">
         <v>12</v>
       </c>
@@ -12118,7 +12112,7 @@
       <c r="J427" s="1"/>
       <c r="K427" s="1"/>
     </row>
-    <row r="428" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" s="11"/>
       <c r="B428" s="11"/>
       <c r="C428" s="12"/>
@@ -12137,11 +12131,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{36663624-9048-4258-8F9E-F8388303C4CD}" showPageBreaks="1" fitToPage="1" showAutoFilter="1" hiddenColumns="1">
-      <selection activeCell="M14" sqref="M14"/>
+    <customSheetView guid="{1E205BAA-3839-4793-9AC9-6DFA286FC573}" showPageBreaks="1" fitToPage="1" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
       <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <printOptions gridLines="1"/>
-      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+      <pageSetup scale="40" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+      <autoFilter ref="A1:J409"/>
+    </customSheetView>
+    <customSheetView guid="{9C0311F0-DF70-44FD-BFCF-C4DBE8DC2CBB}" fitToPage="1" showAutoFilter="1" hiddenColumns="1">
+      <selection activeCell="F11" sqref="F11"/>
+      <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <printOptions gridLines="1"/>
+      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId2"/>
       <autoFilter ref="A1:J366">
         <sortState ref="A2:J366">
           <sortCondition ref="A2:A366"/>
@@ -12151,31 +12153,23 @@
     <customSheetView guid="{FBFDDEB8-09C3-4C2E-8A82-FA3F5F43B9A0}" showPageBreaks="1" fitToPage="1" showAutoFilter="1" hiddenColumns="1">
       <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <printOptions gridLines="1"/>
-      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId3"/>
       <autoFilter ref="A1:J366">
         <sortState ref="A2:J366">
           <sortCondition descending="1" ref="A2:A366"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{9C0311F0-DF70-44FD-BFCF-C4DBE8DC2CBB}" fitToPage="1" showAutoFilter="1" hiddenColumns="1">
-      <selection activeCell="F11" sqref="F11"/>
+    <customSheetView guid="{36663624-9048-4258-8F9E-F8388303C4CD}" showPageBreaks="1" fitToPage="1" showAutoFilter="1" hiddenColumns="1">
+      <selection activeCell="M14" sqref="M14"/>
       <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <printOptions gridLines="1"/>
-      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+      <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId4"/>
       <autoFilter ref="A1:J366">
         <sortState ref="A2:J366">
           <sortCondition ref="A2:A366"/>
         </sortState>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{1E205BAA-3839-4793-9AC9-6DFA286FC573}" showPageBreaks="1" fitToPage="1" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
-      <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <printOptions gridLines="1"/>
-      <pageSetup scale="40" fitToHeight="0" orientation="landscape" r:id="rId4"/>
-      <autoFilter ref="A1:J409"/>
     </customSheetView>
   </customSheetViews>
   <printOptions gridLines="1"/>

</xml_diff>